<commit_message>
radio button and localization dynamic
</commit_message>
<xml_diff>
--- a/U_find_31_12_24.xlsx
+++ b/U_find_31_12_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/external_1/Code/python/office/excel_mapper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atique.hossain\Desktop\excel_mapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C91C8C-2305-BF4F-B86E-D094513A8747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F3D5C-F61D-4FD9-9F6A-F8E18B06E8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19920" activeTab="3" xr2:uid="{98118860-C578-4587-916B-A7E3CA3C03BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{98118860-C578-4587-916B-A7E3CA3C03BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions - Idea Log" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="2001">
   <si>
     <t>#</t>
   </si>
@@ -12155,6 +12155,9 @@
   </si>
   <si>
     <t>aa</t>
+  </si>
+  <si>
+    <t>radio</t>
   </si>
 </sst>
 </file>
@@ -14366,23 +14369,23 @@
       <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="76" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="41" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="76" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="41" customWidth="1"/>
     <col min="3" max="4" width="28" style="20" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="39.83203125" style="42" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" style="43" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" style="41" customWidth="1"/>
+    <col min="8" max="8" width="39.85546875" style="42" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="43" customWidth="1"/>
     <col min="10" max="10" width="42" style="43" customWidth="1"/>
-    <col min="11" max="11" width="31.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="42" style="1" customWidth="1"/>
-    <col min="13" max="13" width="40.5" customWidth="1"/>
+    <col min="13" max="13" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="21" customFormat="1" ht="35.5" customHeight="1">
+    <row r="1" spans="1:12" s="21" customFormat="1" ht="35.450000000000003" customHeight="1">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -14452,7 +14455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="80.5" hidden="1" customHeight="1">
+    <row r="3" spans="1:12" ht="80.45" hidden="1" customHeight="1">
       <c r="A3" s="39" t="s">
         <v>21</v>
       </c>
@@ -14484,7 +14487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="105.5" hidden="1" customHeight="1">
+    <row r="4" spans="1:12" ht="105.6" hidden="1" customHeight="1">
       <c r="A4" s="39" t="s">
         <v>30</v>
       </c>
@@ -14608,7 +14611,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="157" hidden="1" customHeight="1">
+    <row r="8" spans="1:12" ht="156.94999999999999" hidden="1" customHeight="1">
       <c r="A8" s="39" t="s">
         <v>64</v>
       </c>
@@ -14672,7 +14675,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="159.5" hidden="1" customHeight="1">
+    <row r="10" spans="1:12" ht="159.6" hidden="1" customHeight="1">
       <c r="A10" s="39" t="s">
         <v>82</v>
       </c>
@@ -14732,7 +14735,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="99.5" hidden="1" customHeight="1">
+    <row r="12" spans="1:12" ht="99.6" hidden="1" customHeight="1">
       <c r="A12" s="39" t="s">
         <v>98</v>
       </c>
@@ -14788,7 +14791,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="151" hidden="1" customHeight="1">
+    <row r="14" spans="1:12" ht="150.94999999999999" hidden="1" customHeight="1">
       <c r="A14" s="39" t="s">
         <v>112</v>
       </c>
@@ -14918,7 +14921,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="83.5" hidden="1" customHeight="1">
+    <row r="18" spans="1:12" ht="83.45" hidden="1" customHeight="1">
       <c r="A18" s="39" t="s">
         <v>147</v>
       </c>
@@ -15052,7 +15055,7 @@
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="147.5" hidden="1" customHeight="1">
+    <row r="22" spans="1:12" ht="147.6" hidden="1" customHeight="1">
       <c r="A22" s="39" t="s">
         <v>182</v>
       </c>
@@ -17498,30 +17501,30 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="19.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="60" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="62" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="59.1640625" style="60" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" style="60" customWidth="1"/>
-    <col min="8" max="8" width="65.6640625" style="60" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="60" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="60" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="60" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="62" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" style="60" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="60" customWidth="1"/>
+    <col min="8" max="8" width="65.5703125" style="60" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="60" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="60" customWidth="1"/>
     <col min="11" max="11" width="37" style="60" customWidth="1"/>
-    <col min="12" max="12" width="58.1640625" style="60" customWidth="1"/>
-    <col min="13" max="13" width="33.33203125" style="60" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="60"/>
+    <col min="12" max="12" width="58.140625" style="60" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" style="60" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="59" customFormat="1" ht="16">
+    <row r="1" spans="1:13" s="59" customFormat="1" ht="15.75">
       <c r="A1" s="59" t="s">
         <v>813</v>
       </c>
@@ -17562,7 +17565,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:13" customFormat="1" ht="50">
+    <row r="2" spans="1:13" customFormat="1" ht="60">
       <c r="A2" s="288" t="s">
         <v>824</v>
       </c>
@@ -17727,7 +17730,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="9" spans="1:13" customFormat="1" ht="50">
+    <row r="9" spans="1:13" customFormat="1" ht="45">
       <c r="A9" s="289"/>
       <c r="B9" s="116" t="s">
         <v>270</v>
@@ -17764,7 +17767,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="10" spans="1:13" customFormat="1" ht="32">
+    <row r="10" spans="1:13" customFormat="1" ht="15.75">
       <c r="A10" s="289"/>
       <c r="B10" s="114"/>
       <c r="C10" s="115"/>
@@ -17787,7 +17790,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="11" spans="1:13" customFormat="1" ht="32">
+    <row r="11" spans="1:13" customFormat="1" ht="30">
       <c r="A11" s="289"/>
       <c r="B11" s="114"/>
       <c r="C11" s="115"/>
@@ -17810,7 +17813,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="12" spans="1:13" customFormat="1" ht="16">
+    <row r="12" spans="1:13" customFormat="1" ht="15.75">
       <c r="A12" s="289"/>
       <c r="B12" s="114"/>
       <c r="C12" s="115"/>
@@ -17831,7 +17834,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="13" spans="1:13" customFormat="1" ht="32">
+    <row r="13" spans="1:13" customFormat="1" ht="30">
       <c r="A13" s="289"/>
       <c r="B13" s="114"/>
       <c r="C13" s="115"/>
@@ -17852,7 +17855,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="14" spans="1:13" customFormat="1" ht="16">
+    <row r="14" spans="1:13" customFormat="1" ht="15.75">
       <c r="A14" s="289"/>
       <c r="B14" s="114"/>
       <c r="C14" s="115"/>
@@ -17873,7 +17876,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="15" spans="1:13" customFormat="1" ht="32">
+    <row r="15" spans="1:13" customFormat="1" ht="15.75">
       <c r="A15" s="289"/>
       <c r="B15" s="114"/>
       <c r="C15" s="115"/>
@@ -17894,7 +17897,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="16" spans="1:13" customFormat="1" ht="16">
+    <row r="16" spans="1:13" customFormat="1" ht="15.75">
       <c r="A16" s="289"/>
       <c r="B16" s="114"/>
       <c r="C16" s="115"/>
@@ -17915,7 +17918,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="17" spans="1:13" customFormat="1" ht="16">
+    <row r="17" spans="1:13" customFormat="1" ht="15.75">
       <c r="A17" s="289"/>
       <c r="B17" s="114"/>
       <c r="C17" s="115"/>
@@ -17936,7 +17939,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="18" spans="1:13" customFormat="1" ht="32">
+    <row r="18" spans="1:13" customFormat="1" ht="15.75">
       <c r="A18" s="289"/>
       <c r="B18" s="114"/>
       <c r="C18" s="115"/>
@@ -17957,7 +17960,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="19" spans="1:13" customFormat="1" ht="16">
+    <row r="19" spans="1:13" customFormat="1" ht="15.75">
       <c r="A19" s="289"/>
       <c r="B19" s="114"/>
       <c r="C19" s="115"/>
@@ -17978,7 +17981,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="20" spans="1:13" customFormat="1" ht="48">
+    <row r="20" spans="1:13" customFormat="1" ht="45">
       <c r="A20" s="289"/>
       <c r="B20" s="114" t="s">
         <v>280</v>
@@ -18015,7 +18018,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="21" spans="1:13" customFormat="1" ht="16">
+    <row r="21" spans="1:13" customFormat="1" ht="15.75">
       <c r="A21" s="289"/>
       <c r="B21" s="114"/>
       <c r="C21" s="115"/>
@@ -18036,7 +18039,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:13" customFormat="1" ht="16">
+    <row r="22" spans="1:13" customFormat="1" ht="15.75">
       <c r="A22" s="289"/>
       <c r="B22" s="114"/>
       <c r="C22" s="115"/>
@@ -18057,7 +18060,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="23" spans="1:13" customFormat="1" ht="16">
+    <row r="23" spans="1:13" customFormat="1" ht="15.75">
       <c r="A23" s="289"/>
       <c r="B23" s="114"/>
       <c r="C23" s="115"/>
@@ -18078,7 +18081,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="24" spans="1:13" customFormat="1" ht="16">
+    <row r="24" spans="1:13" customFormat="1" ht="15.75">
       <c r="A24" s="289"/>
       <c r="B24" s="114"/>
       <c r="C24" s="115"/>
@@ -18099,7 +18102,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="25" spans="1:13" customFormat="1" ht="16">
+    <row r="25" spans="1:13" customFormat="1" ht="15.75">
       <c r="A25" s="289"/>
       <c r="B25" s="114"/>
       <c r="C25" s="115"/>
@@ -18120,7 +18123,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="26" spans="1:13" customFormat="1" ht="16">
+    <row r="26" spans="1:13" customFormat="1" ht="15.75">
       <c r="A26" s="289"/>
       <c r="B26" s="114"/>
       <c r="C26" s="115"/>
@@ -18141,7 +18144,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="27" spans="1:13" customFormat="1" ht="16">
+    <row r="27" spans="1:13" customFormat="1" ht="15.75">
       <c r="A27" s="289"/>
       <c r="B27" s="114"/>
       <c r="C27" s="115"/>
@@ -18162,7 +18165,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="28" spans="1:13" customFormat="1" ht="16">
+    <row r="28" spans="1:13" customFormat="1" ht="15.75">
       <c r="A28" s="289"/>
       <c r="B28" s="114"/>
       <c r="C28" s="115"/>
@@ -18183,7 +18186,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="29" spans="1:13" customFormat="1" ht="16">
+    <row r="29" spans="1:13" customFormat="1" ht="15.75">
       <c r="A29" s="289"/>
       <c r="B29" s="114"/>
       <c r="C29" s="115"/>
@@ -18204,7 +18207,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="30" spans="1:13" customFormat="1" ht="16">
+    <row r="30" spans="1:13" customFormat="1" ht="15.75">
       <c r="A30" s="289"/>
       <c r="B30" s="114"/>
       <c r="C30" s="115"/>
@@ -18225,7 +18228,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="31" spans="1:13" customFormat="1" ht="16">
+    <row r="31" spans="1:13" customFormat="1" ht="15.75">
       <c r="A31" s="289"/>
       <c r="B31" s="114"/>
       <c r="C31" s="115"/>
@@ -18246,7 +18249,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="32" spans="1:13" customFormat="1" ht="16">
+    <row r="32" spans="1:13" customFormat="1" ht="15.75">
       <c r="A32" s="289"/>
       <c r="B32" s="114"/>
       <c r="C32" s="115"/>
@@ -18267,7 +18270,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="33" spans="1:16" customFormat="1" ht="16">
+    <row r="33" spans="1:16" customFormat="1" ht="15.75">
       <c r="A33" s="289"/>
       <c r="B33" s="114"/>
       <c r="C33" s="115"/>
@@ -18288,7 +18291,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="34" spans="1:16" customFormat="1" ht="16">
+    <row r="34" spans="1:16" customFormat="1" ht="15.75">
       <c r="A34" s="289"/>
       <c r="B34" s="114"/>
       <c r="C34" s="115"/>
@@ -18309,7 +18312,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="35" spans="1:16" customFormat="1" ht="16">
+    <row r="35" spans="1:16" customFormat="1" ht="15.75">
       <c r="A35" s="289"/>
       <c r="B35" s="114"/>
       <c r="C35" s="115"/>
@@ -18330,7 +18333,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="36" spans="1:16" customFormat="1" ht="16">
+    <row r="36" spans="1:16" customFormat="1" ht="15.75">
       <c r="A36" s="289"/>
       <c r="B36" s="114"/>
       <c r="C36" s="115"/>
@@ -18351,7 +18354,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="37" spans="1:16" customFormat="1" ht="16">
+    <row r="37" spans="1:16" customFormat="1" ht="15.75">
       <c r="A37" s="289"/>
       <c r="B37" s="114"/>
       <c r="C37" s="115"/>
@@ -18372,7 +18375,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="38" spans="1:16" customFormat="1" ht="16">
+    <row r="38" spans="1:16" customFormat="1" ht="15.75">
       <c r="A38" s="290"/>
       <c r="B38" s="114"/>
       <c r="C38" s="115"/>
@@ -18453,7 +18456,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="41" spans="1:16" customFormat="1" ht="34">
+    <row r="41" spans="1:16" customFormat="1" ht="30">
       <c r="A41" s="289"/>
       <c r="B41" s="114" t="s">
         <v>296</v>
@@ -18490,7 +18493,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="42" spans="1:16" customFormat="1" ht="18">
+    <row r="42" spans="1:16" customFormat="1" ht="15.75">
       <c r="A42" s="289"/>
       <c r="B42" s="114"/>
       <c r="C42" s="115"/>
@@ -18511,7 +18514,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="43" spans="1:16" customFormat="1" ht="18">
+    <row r="43" spans="1:16" customFormat="1" ht="15.75">
       <c r="A43" s="289"/>
       <c r="B43" s="114"/>
       <c r="C43" s="115"/>
@@ -18535,7 +18538,7 @@
       <c r="O43" s="172"/>
       <c r="P43" s="172"/>
     </row>
-    <row r="44" spans="1:16" customFormat="1" ht="18">
+    <row r="44" spans="1:16" customFormat="1" ht="15.75">
       <c r="A44" s="289"/>
       <c r="B44" s="114"/>
       <c r="C44" s="115"/>
@@ -18559,7 +18562,7 @@
       <c r="O44" s="172"/>
       <c r="P44" s="172"/>
     </row>
-    <row r="45" spans="1:16" customFormat="1" ht="18">
+    <row r="45" spans="1:16" customFormat="1" ht="15.75">
       <c r="A45" s="289"/>
       <c r="B45" s="114"/>
       <c r="C45" s="115"/>
@@ -18583,7 +18586,7 @@
       <c r="O45" s="172"/>
       <c r="P45" s="172"/>
     </row>
-    <row r="46" spans="1:16" customFormat="1" ht="18">
+    <row r="46" spans="1:16" customFormat="1" ht="15.75">
       <c r="A46" s="289"/>
       <c r="B46" s="114"/>
       <c r="C46" s="115"/>
@@ -18607,7 +18610,7 @@
       <c r="O46" s="172"/>
       <c r="P46" s="172"/>
     </row>
-    <row r="47" spans="1:16" customFormat="1" ht="18">
+    <row r="47" spans="1:16" customFormat="1" ht="15.75">
       <c r="A47" s="289"/>
       <c r="B47" s="114"/>
       <c r="C47" s="115"/>
@@ -18628,7 +18631,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="48" spans="1:16" customFormat="1" ht="18">
+    <row r="48" spans="1:16" customFormat="1" ht="15.75">
       <c r="A48" s="289"/>
       <c r="B48" s="114"/>
       <c r="C48" s="115"/>
@@ -18649,7 +18652,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="49" spans="1:13" customFormat="1" ht="18">
+    <row r="49" spans="1:13" customFormat="1" ht="15.75">
       <c r="A49" s="289"/>
       <c r="B49" s="114"/>
       <c r="C49" s="115"/>
@@ -18670,7 +18673,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="50" spans="1:13" customFormat="1" ht="18">
+    <row r="50" spans="1:13" customFormat="1" ht="15.75">
       <c r="A50" s="289"/>
       <c r="B50" s="114"/>
       <c r="C50" s="115"/>
@@ -18691,7 +18694,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="51" spans="1:13" customFormat="1" ht="18">
+    <row r="51" spans="1:13" customFormat="1" ht="15.75">
       <c r="A51" s="289"/>
       <c r="B51" s="114"/>
       <c r="C51" s="115"/>
@@ -18712,7 +18715,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" spans="1:13" customFormat="1" ht="18">
+    <row r="52" spans="1:13" customFormat="1" ht="15.75">
       <c r="A52" s="290"/>
       <c r="B52" s="114"/>
       <c r="C52" s="115"/>
@@ -18772,7 +18775,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="54" spans="1:13" customFormat="1" ht="16">
+    <row r="54" spans="1:13" customFormat="1" ht="15">
       <c r="A54" s="291"/>
       <c r="B54" s="140"/>
       <c r="C54" s="179"/>
@@ -18793,7 +18796,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="55" spans="1:13" customFormat="1" ht="82">
+    <row r="55" spans="1:13" customFormat="1" ht="105">
       <c r="A55" s="292"/>
       <c r="B55" s="114" t="s">
         <v>393</v>
@@ -18832,7 +18835,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="56" spans="1:13" customFormat="1" ht="15">
+    <row r="56" spans="1:13" customFormat="1" ht="15.75">
       <c r="A56" s="292"/>
       <c r="B56" s="70"/>
       <c r="C56" s="67"/>
@@ -18895,7 +18898,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="32">
+    <row r="59" spans="1:13" ht="45.75">
       <c r="A59" s="289"/>
       <c r="B59" s="121" t="s">
         <v>524</v>
@@ -18932,7 +18935,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="16">
+    <row r="60" spans="1:13" ht="15.75">
       <c r="A60" s="289"/>
       <c r="B60" s="121"/>
       <c r="C60" s="114"/>
@@ -18953,7 +18956,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="16">
+    <row r="61" spans="1:13" ht="15.75">
       <c r="A61" s="289"/>
       <c r="B61" s="121"/>
       <c r="C61" s="114"/>
@@ -18974,7 +18977,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="16">
+    <row r="62" spans="1:13" ht="15.75">
       <c r="A62" s="289"/>
       <c r="B62" s="121"/>
       <c r="C62" s="114"/>
@@ -18995,7 +18998,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="16">
+    <row r="63" spans="1:13" ht="15.75">
       <c r="A63" s="289"/>
       <c r="B63" s="121"/>
       <c r="C63" s="114"/>
@@ -19016,7 +19019,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="16">
+    <row r="64" spans="1:13" ht="15.75">
       <c r="A64" s="289"/>
       <c r="B64" s="121"/>
       <c r="C64" s="114"/>
@@ -19037,7 +19040,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="16">
+    <row r="65" spans="1:13" ht="15.75">
       <c r="A65" s="289"/>
       <c r="B65" s="121"/>
       <c r="C65" s="114"/>
@@ -19058,7 +19061,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="16">
+    <row r="66" spans="1:13" ht="15.75">
       <c r="A66" s="289"/>
       <c r="B66" s="121"/>
       <c r="C66" s="114"/>
@@ -19079,7 +19082,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="16">
+    <row r="67" spans="1:13" ht="15.75">
       <c r="A67" s="289"/>
       <c r="B67" s="121"/>
       <c r="C67" s="114"/>
@@ -19100,7 +19103,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="16">
+    <row r="68" spans="1:13" ht="30">
       <c r="A68" s="289"/>
       <c r="B68" s="121"/>
       <c r="C68" s="114"/>
@@ -19121,7 +19124,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="16">
+    <row r="69" spans="1:13" ht="15.75">
       <c r="A69" s="289"/>
       <c r="B69" s="121"/>
       <c r="C69" s="114"/>
@@ -19142,7 +19145,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="16">
+    <row r="70" spans="1:13" ht="30">
       <c r="A70" s="289"/>
       <c r="B70" s="121"/>
       <c r="C70" s="114"/>
@@ -19163,7 +19166,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="48">
+    <row r="71" spans="1:13" ht="45">
       <c r="A71" s="289"/>
       <c r="B71" s="121"/>
       <c r="C71" s="114"/>
@@ -19184,7 +19187,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="192">
+    <row r="72" spans="1:13" ht="210">
       <c r="A72" s="289"/>
       <c r="B72" s="121" t="s">
         <v>542</v>
@@ -19223,7 +19226,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="16">
+    <row r="73" spans="1:13" ht="15">
       <c r="A73" s="289"/>
       <c r="B73" s="114"/>
       <c r="C73" s="114"/>
@@ -19244,7 +19247,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="192">
+    <row r="74" spans="1:13" ht="210">
       <c r="A74" s="289"/>
       <c r="B74" s="121" t="s">
         <v>552</v>
@@ -19277,7 +19280,7 @@
       <c r="L74" s="114"/>
       <c r="M74" s="114"/>
     </row>
-    <row r="75" spans="1:13" ht="192">
+    <row r="75" spans="1:13" ht="210">
       <c r="A75" s="290"/>
       <c r="B75" s="121" t="s">
         <v>561</v>
@@ -19310,7 +19313,7 @@
       <c r="L75" s="114"/>
       <c r="M75" s="114"/>
     </row>
-    <row r="76" spans="1:13" ht="128">
+    <row r="76" spans="1:13" ht="150">
       <c r="A76" s="293" t="s">
         <v>1075</v>
       </c>
@@ -19351,7 +19354,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="16">
+    <row r="77" spans="1:13" ht="15.75">
       <c r="A77" s="293"/>
       <c r="B77" s="121"/>
       <c r="C77" s="114"/>
@@ -19372,7 +19375,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="48">
+    <row r="78" spans="1:13" ht="45">
       <c r="A78" s="293"/>
       <c r="B78" s="141"/>
       <c r="C78" s="140" t="s">
@@ -19403,7 +19406,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16">
+    <row r="79" spans="1:13" ht="15.75">
       <c r="A79" s="293"/>
       <c r="B79" s="141"/>
       <c r="C79" s="140"/>
@@ -19424,7 +19427,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="16">
+    <row r="80" spans="1:13" ht="15.75">
       <c r="A80" s="293"/>
       <c r="B80" s="141"/>
       <c r="C80" s="140"/>
@@ -19445,7 +19448,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="16">
+    <row r="81" spans="1:16" ht="15.75">
       <c r="A81" s="293"/>
       <c r="B81" s="141"/>
       <c r="C81" s="140"/>
@@ -19466,7 +19469,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="16">
+    <row r="82" spans="1:16" ht="15.75">
       <c r="A82" s="293"/>
       <c r="B82" s="141"/>
       <c r="C82" s="140"/>
@@ -19487,7 +19490,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="16">
+    <row r="83" spans="1:16" ht="15.75">
       <c r="A83" s="293"/>
       <c r="B83" s="141"/>
       <c r="C83" s="140"/>
@@ -19508,7 +19511,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="16">
+    <row r="84" spans="1:16" ht="15.75">
       <c r="A84" s="293"/>
       <c r="B84" s="141"/>
       <c r="C84" s="140"/>
@@ -19529,7 +19532,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="16">
+    <row r="85" spans="1:16" ht="15.75">
       <c r="A85" s="293"/>
       <c r="B85" s="141"/>
       <c r="C85" s="140"/>
@@ -19550,7 +19553,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="16">
+    <row r="86" spans="1:16" ht="15.75">
       <c r="A86" s="293"/>
       <c r="B86" s="141"/>
       <c r="C86" s="140"/>
@@ -19571,7 +19574,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="16">
+    <row r="87" spans="1:16" ht="15.75">
       <c r="A87" s="293"/>
       <c r="B87" s="141"/>
       <c r="C87" s="140"/>
@@ -19592,7 +19595,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="16">
+    <row r="88" spans="1:16" ht="15.75">
       <c r="A88" s="293"/>
       <c r="B88" s="141"/>
       <c r="C88" s="140"/>
@@ -19613,7 +19616,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="16">
+    <row r="89" spans="1:16" ht="15.75">
       <c r="A89" s="293"/>
       <c r="B89" s="141"/>
       <c r="C89" s="140"/>
@@ -19634,7 +19637,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="16">
+    <row r="90" spans="1:16" ht="15.75">
       <c r="A90" s="293"/>
       <c r="B90" s="141"/>
       <c r="C90" s="140"/>
@@ -19655,7 +19658,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="16">
+    <row r="91" spans="1:16" ht="15.75">
       <c r="A91" s="293"/>
       <c r="B91" s="141"/>
       <c r="C91" s="140"/>
@@ -19676,7 +19679,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="16">
+    <row r="92" spans="1:16" ht="15.75">
       <c r="A92" s="293"/>
       <c r="B92" s="141"/>
       <c r="C92" s="140"/>
@@ -19697,7 +19700,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="16">
+    <row r="93" spans="1:16" ht="15.75">
       <c r="A93" s="293"/>
       <c r="B93" s="141"/>
       <c r="C93" s="140"/>
@@ -19718,7 +19721,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="64" customFormat="1" ht="48">
+    <row r="94" spans="1:16" s="64" customFormat="1" ht="45.75">
       <c r="A94" s="285"/>
       <c r="B94" s="71" t="s">
         <v>704</v>
@@ -19820,7 +19823,7 @@
       <c r="O96" s="108"/>
       <c r="P96" s="108"/>
     </row>
-    <row r="97" spans="1:13" ht="15">
+    <row r="97" spans="1:13" ht="15.75">
       <c r="A97" s="140"/>
       <c r="B97" s="141"/>
       <c r="C97" s="140"/>
@@ -19904,25 +19907,24 @@
       <selection pane="topRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
-    <col min="4" max="4" width="39.5" style="60" customWidth="1"/>
-    <col min="5" max="5" width="52.5" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="42" customWidth="1"/>
-    <col min="7" max="7" width="38.33203125" style="42" customWidth="1"/>
-    <col min="8" max="8" width="35.5" style="42" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="42" customWidth="1"/>
-    <col min="10" max="10" width="25.5" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" customWidth="1"/>
-    <col min="12" max="12" width="67.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="7" width="38.42578125" style="42" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" style="42" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="42" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="67.5703125" customWidth="1"/>
     <col min="13" max="13" width="73" customWidth="1"/>
-    <col min="14" max="14" width="108.83203125" customWidth="1"/>
+    <col min="14" max="14" width="108.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="81" t="s">
         <v>813</v>
       </c>
@@ -19966,7 +19968,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39">
+    <row r="2" spans="1:14" ht="38.25">
       <c r="A2" s="295" t="s">
         <v>1150</v>
       </c>
@@ -20124,7 +20126,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16">
+    <row r="7" spans="1:14" ht="15.75">
       <c r="A7" s="295"/>
       <c r="B7" s="83"/>
       <c r="C7" s="193"/>
@@ -20146,7 +20148,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16">
+    <row r="8" spans="1:14" ht="15.75">
       <c r="A8" s="295"/>
       <c r="B8" s="83"/>
       <c r="C8" s="193"/>
@@ -20168,7 +20170,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16">
+    <row r="9" spans="1:14" ht="15.75">
       <c r="A9" s="295"/>
       <c r="B9" s="83"/>
       <c r="C9" s="193"/>
@@ -20190,7 +20192,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16">
+    <row r="10" spans="1:14" ht="15.75">
       <c r="A10" s="295"/>
       <c r="B10" s="83"/>
       <c r="C10" s="193"/>
@@ -20212,7 +20214,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16">
+    <row r="11" spans="1:14" ht="15.75">
       <c r="A11" s="295"/>
       <c r="B11" s="83"/>
       <c r="C11" s="193"/>
@@ -20234,7 +20236,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16">
+    <row r="12" spans="1:14" ht="15.75">
       <c r="A12" s="295"/>
       <c r="B12" s="83"/>
       <c r="C12" s="193"/>
@@ -20256,7 +20258,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="75">
+    <row r="13" spans="1:14" ht="67.5">
       <c r="A13" s="295"/>
       <c r="B13" s="83" t="s">
         <v>457</v>
@@ -20364,7 +20366,7 @@
       <c r="M16" s="68"/>
       <c r="N16" s="68"/>
     </row>
-    <row r="17" spans="1:14" ht="65">
+    <row r="17" spans="1:14" ht="51">
       <c r="A17" s="296" t="s">
         <v>1211</v>
       </c>
@@ -20408,7 +20410,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16">
+    <row r="18" spans="1:14">
       <c r="A18" s="296"/>
       <c r="B18" s="68"/>
       <c r="C18" s="68"/>
@@ -20468,7 +20470,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="19">
+    <row r="20" spans="1:14" ht="19.5">
       <c r="A20" s="296"/>
       <c r="B20" s="83"/>
       <c r="C20" s="193"/>
@@ -20490,7 +20492,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="19">
+    <row r="21" spans="1:14" ht="19.5">
       <c r="A21" s="296"/>
       <c r="B21" s="83"/>
       <c r="C21" s="193"/>
@@ -20512,7 +20514,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="19">
+    <row r="22" spans="1:14" ht="19.5">
       <c r="A22" s="296"/>
       <c r="B22" s="83"/>
       <c r="C22" s="193"/>
@@ -20534,7 +20536,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="19">
+    <row r="23" spans="1:14" ht="19.5">
       <c r="A23" s="296"/>
       <c r="B23" s="83"/>
       <c r="C23" s="193"/>
@@ -20556,7 +20558,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="19">
+    <row r="24" spans="1:14" ht="19.5">
       <c r="A24" s="296"/>
       <c r="B24" s="83"/>
       <c r="C24" s="193"/>
@@ -20578,7 +20580,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="45">
+    <row r="25" spans="1:14" ht="58.5">
       <c r="A25" s="296"/>
       <c r="B25" s="83"/>
       <c r="C25" s="193"/>
@@ -20604,7 +20606,7 @@
       <c r="M25" s="68"/>
       <c r="N25" s="68"/>
     </row>
-    <row r="26" spans="1:14" ht="96">
+    <row r="26" spans="1:14" ht="90">
       <c r="A26" s="297" t="s">
         <v>1245</v>
       </c>
@@ -20648,7 +20650,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16">
+    <row r="27" spans="1:14">
       <c r="A27" s="296"/>
       <c r="B27" s="68"/>
       <c r="C27" s="68"/>
@@ -20670,7 +20672,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="117">
+    <row r="28" spans="1:14" ht="102">
       <c r="A28" s="296"/>
       <c r="B28" s="83" t="s">
         <v>499</v>
@@ -20708,7 +20710,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16">
+    <row r="29" spans="1:14" ht="15.75">
       <c r="A29" s="296"/>
       <c r="B29" s="83"/>
       <c r="C29" s="193"/>
@@ -20730,7 +20732,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16">
+    <row r="30" spans="1:14" ht="15.75">
       <c r="A30" s="296"/>
       <c r="B30" s="83"/>
       <c r="C30" s="193"/>
@@ -20752,7 +20754,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16">
+    <row r="31" spans="1:14" ht="15.75">
       <c r="A31" s="296"/>
       <c r="B31" s="83"/>
       <c r="C31" s="193"/>
@@ -20774,7 +20776,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16">
+    <row r="32" spans="1:14" ht="15.75">
       <c r="A32" s="296"/>
       <c r="B32" s="68"/>
       <c r="C32" s="68"/>
@@ -20867,7 +20869,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="16">
+    <row r="35" spans="1:16">
       <c r="A35" s="295"/>
       <c r="B35" s="68"/>
       <c r="C35" s="68"/>
@@ -20927,7 +20929,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="16">
+    <row r="37" spans="1:16" ht="15.75">
       <c r="A37" s="295"/>
       <c r="B37" s="83"/>
       <c r="C37" s="193"/>
@@ -20949,7 +20951,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="16">
+    <row r="38" spans="1:16" ht="15.75">
       <c r="A38" s="295"/>
       <c r="B38" s="83"/>
       <c r="C38" s="193"/>
@@ -20971,7 +20973,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="16">
+    <row r="39" spans="1:16" ht="15.75">
       <c r="A39" s="295"/>
       <c r="B39" s="83"/>
       <c r="C39" s="193"/>
@@ -20993,7 +20995,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="16">
+    <row r="40" spans="1:16" ht="15.75">
       <c r="A40" s="295"/>
       <c r="B40" s="83"/>
       <c r="C40" s="193"/>
@@ -21015,7 +21017,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="16">
+    <row r="41" spans="1:16" ht="15.75">
       <c r="A41" s="295"/>
       <c r="B41" s="83"/>
       <c r="C41" s="193"/>
@@ -21037,7 +21039,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="60">
+    <row r="42" spans="1:16" ht="56.25">
       <c r="A42" s="295" t="s">
         <v>1303</v>
       </c>
@@ -21077,7 +21079,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="16">
+    <row r="43" spans="1:16" ht="15.75">
       <c r="A43" s="295"/>
       <c r="B43" s="83"/>
       <c r="C43" s="193"/>
@@ -21099,7 +21101,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="16">
+    <row r="44" spans="1:16" ht="15.75">
       <c r="A44" s="295"/>
       <c r="B44" s="83"/>
       <c r="C44" s="193"/>
@@ -21121,7 +21123,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="16">
+    <row r="45" spans="1:16" ht="15.75">
       <c r="A45" s="295"/>
       <c r="B45" s="83"/>
       <c r="C45" s="193"/>
@@ -21143,7 +21145,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16">
+    <row r="46" spans="1:16" ht="15.75">
       <c r="A46" s="295"/>
       <c r="B46" s="83"/>
       <c r="C46" s="193"/>
@@ -21165,7 +21167,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16">
+    <row r="47" spans="1:16" ht="15.75">
       <c r="A47" s="295"/>
       <c r="B47" s="83"/>
       <c r="C47" s="193"/>
@@ -21187,7 +21189,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="16">
+    <row r="48" spans="1:16" ht="15.75">
       <c r="A48" s="295"/>
       <c r="B48" s="83"/>
       <c r="C48" s="193"/>
@@ -21209,7 +21211,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16">
+    <row r="49" spans="1:14" ht="15.75">
       <c r="A49" s="295"/>
       <c r="B49" s="83"/>
       <c r="C49" s="193"/>
@@ -21231,7 +21233,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16">
+    <row r="50" spans="1:14" ht="15.75">
       <c r="A50" s="295"/>
       <c r="B50" s="83"/>
       <c r="C50" s="193"/>
@@ -21253,7 +21255,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16">
+    <row r="51" spans="1:14" ht="15.75">
       <c r="A51" s="295"/>
       <c r="B51" s="83"/>
       <c r="C51" s="193"/>
@@ -21275,7 +21277,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="48">
+    <row r="52" spans="1:14" ht="45">
       <c r="A52" s="295"/>
       <c r="B52" s="83" t="s">
         <v>579</v>
@@ -21313,7 +21315,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16">
+    <row r="53" spans="1:14" ht="15.75">
       <c r="A53" s="295"/>
       <c r="B53" s="83"/>
       <c r="C53" s="193"/>
@@ -21335,7 +21337,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="16">
+    <row r="54" spans="1:14" ht="15.75">
       <c r="A54" s="295"/>
       <c r="B54" s="83"/>
       <c r="C54" s="193"/>
@@ -21357,7 +21359,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="16">
+    <row r="55" spans="1:14" ht="15.75">
       <c r="A55" s="295"/>
       <c r="B55" s="83"/>
       <c r="C55" s="193"/>
@@ -21379,7 +21381,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16">
+    <row r="56" spans="1:14" ht="15.75">
       <c r="A56" s="295"/>
       <c r="B56" s="83"/>
       <c r="C56" s="193"/>
@@ -21401,7 +21403,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="16">
+    <row r="57" spans="1:14" ht="15.75">
       <c r="A57" s="295"/>
       <c r="B57" s="83"/>
       <c r="C57" s="193"/>
@@ -21423,7 +21425,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16">
+    <row r="58" spans="1:14" ht="15.75">
       <c r="A58" s="295"/>
       <c r="B58" s="83"/>
       <c r="C58" s="193"/>
@@ -21445,7 +21447,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="16">
+    <row r="59" spans="1:14" ht="15.75">
       <c r="A59" s="295"/>
       <c r="B59" s="68"/>
       <c r="C59" s="66" t="s">
@@ -21531,7 +21533,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="16">
+    <row r="62" spans="1:14" ht="15.75">
       <c r="A62" s="295"/>
       <c r="B62" s="83"/>
       <c r="C62" s="193"/>
@@ -21553,7 +21555,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="16">
+    <row r="63" spans="1:14" ht="15.75">
       <c r="A63" s="295"/>
       <c r="B63" s="83"/>
       <c r="C63" s="193"/>
@@ -21575,7 +21577,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="16">
+    <row r="64" spans="1:14" ht="15.75">
       <c r="A64" s="295"/>
       <c r="B64" s="83"/>
       <c r="C64" s="193"/>
@@ -21597,7 +21599,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="16">
+    <row r="65" spans="1:14" ht="15.75">
       <c r="A65" s="295"/>
       <c r="B65" s="83"/>
       <c r="C65" s="193"/>
@@ -21619,7 +21621,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="26">
+    <row r="66" spans="1:14" ht="25.5">
       <c r="A66" s="295"/>
       <c r="B66" s="83"/>
       <c r="C66" s="193" t="s">
@@ -21683,7 +21685,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="16">
+    <row r="68" spans="1:14" ht="15.75">
       <c r="A68" s="295"/>
       <c r="B68" s="83"/>
       <c r="C68" s="193"/>
@@ -21705,7 +21707,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="16">
+    <row r="69" spans="1:14" ht="15.75">
       <c r="A69" s="295"/>
       <c r="B69" s="83"/>
       <c r="C69" s="193"/>
@@ -21727,7 +21729,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="16">
+    <row r="70" spans="1:14" ht="15.75">
       <c r="A70" s="295"/>
       <c r="B70" s="83"/>
       <c r="C70" s="193"/>
@@ -21749,7 +21751,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="16">
+    <row r="71" spans="1:14" ht="15.75">
       <c r="A71" s="295"/>
       <c r="B71" s="83"/>
       <c r="C71" s="193"/>
@@ -21771,7 +21773,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="16">
+    <row r="72" spans="1:14" ht="15.75">
       <c r="A72" s="295"/>
       <c r="B72" s="83"/>
       <c r="C72" s="193"/>
@@ -21793,7 +21795,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="16">
+    <row r="73" spans="1:14" ht="15.75">
       <c r="A73" s="295"/>
       <c r="B73" s="83"/>
       <c r="C73" s="193"/>
@@ -21815,7 +21817,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="16">
+    <row r="74" spans="1:14" ht="15.75">
       <c r="A74" s="295"/>
       <c r="B74" s="83"/>
       <c r="C74" s="193"/>
@@ -21875,7 +21877,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="16">
+    <row r="76" spans="1:14" ht="15.75">
       <c r="A76" s="295"/>
       <c r="B76" s="83"/>
       <c r="C76" s="193"/>
@@ -21935,7 +21937,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="16">
+    <row r="78" spans="1:14">
       <c r="A78" s="295"/>
       <c r="B78" s="83"/>
       <c r="C78" s="83"/>
@@ -21957,7 +21959,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="32">
+    <row r="79" spans="1:14" ht="30">
       <c r="A79" s="295"/>
       <c r="B79" s="83" t="s">
         <v>623</v>
@@ -21995,7 +21997,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="17">
+    <row r="80" spans="1:14">
       <c r="A80" s="295"/>
       <c r="B80" s="83"/>
       <c r="C80" s="193"/>
@@ -22016,7 +22018,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="17">
+    <row r="81" spans="1:14">
       <c r="A81" s="295"/>
       <c r="B81" s="83"/>
       <c r="C81" s="193"/>
@@ -22075,7 +22077,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="16">
+    <row r="83" spans="1:14" ht="15.75">
       <c r="A83" s="295"/>
       <c r="B83" s="83"/>
       <c r="C83" s="193"/>
@@ -22097,7 +22099,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="16">
+    <row r="84" spans="1:14" ht="15.75">
       <c r="A84" s="295"/>
       <c r="B84" s="83"/>
       <c r="C84" s="193"/>
@@ -22119,7 +22121,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="16">
+    <row r="85" spans="1:14" ht="15.75">
       <c r="A85" s="295"/>
       <c r="B85" s="83"/>
       <c r="C85" s="193"/>
@@ -22141,7 +22143,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="16">
+    <row r="86" spans="1:14" ht="15.75">
       <c r="A86" s="295"/>
       <c r="B86" s="83"/>
       <c r="C86" s="193"/>
@@ -22163,7 +22165,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="16">
+    <row r="87" spans="1:14" ht="15.75">
       <c r="A87" s="295"/>
       <c r="B87" s="83"/>
       <c r="C87" s="193"/>
@@ -22185,7 +22187,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="16">
+    <row r="88" spans="1:14" ht="15.75">
       <c r="A88" s="295"/>
       <c r="B88" s="83"/>
       <c r="C88" s="193"/>
@@ -22207,7 +22209,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="16">
+    <row r="89" spans="1:14" ht="15.75">
       <c r="A89" s="295"/>
       <c r="B89" s="83"/>
       <c r="C89" s="193"/>
@@ -22229,7 +22231,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="16">
+    <row r="90" spans="1:14" ht="15.75">
       <c r="A90" s="295"/>
       <c r="B90" s="83"/>
       <c r="C90" s="193"/>
@@ -22251,7 +22253,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="16">
+    <row r="91" spans="1:14" ht="15.75">
       <c r="A91" s="295"/>
       <c r="B91" s="83"/>
       <c r="C91" s="193"/>
@@ -22273,7 +22275,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="16">
+    <row r="92" spans="1:14" ht="15.75">
       <c r="A92" s="295"/>
       <c r="B92" s="83"/>
       <c r="C92" s="193"/>
@@ -22295,7 +22297,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="96">
+    <row r="93" spans="1:14" ht="90">
       <c r="A93" s="295"/>
       <c r="B93" s="83" t="s">
         <v>641</v>
@@ -22333,7 +22335,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="16">
+    <row r="94" spans="1:14">
       <c r="A94" s="295"/>
       <c r="B94" s="68"/>
       <c r="C94" s="68"/>
@@ -22393,7 +22395,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="16">
+    <row r="96" spans="1:14" ht="15.75">
       <c r="A96" s="295"/>
       <c r="B96" s="83"/>
       <c r="C96" s="193"/>
@@ -22415,7 +22417,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="16">
+    <row r="97" spans="1:14" ht="15.75">
       <c r="A97" s="295"/>
       <c r="B97" s="83"/>
       <c r="C97" s="193"/>
@@ -22437,7 +22439,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="16">
+    <row r="98" spans="1:14" ht="15.75">
       <c r="A98" s="295"/>
       <c r="B98" s="83"/>
       <c r="C98" s="193"/>
@@ -22459,7 +22461,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="16">
+    <row r="99" spans="1:14" ht="15.75">
       <c r="A99" s="295"/>
       <c r="B99" s="83"/>
       <c r="C99" s="193"/>
@@ -22481,7 +22483,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="16">
+    <row r="100" spans="1:14" ht="15.75">
       <c r="A100" s="295"/>
       <c r="B100" s="83"/>
       <c r="C100" s="193"/>
@@ -22541,7 +22543,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="16">
+    <row r="102" spans="1:14" ht="15.75">
       <c r="A102" s="295"/>
       <c r="B102" s="83"/>
       <c r="C102" s="193"/>
@@ -22563,7 +22565,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="16">
+    <row r="103" spans="1:14" ht="15.75">
       <c r="A103" s="295"/>
       <c r="B103" s="83"/>
       <c r="C103" s="193"/>
@@ -22585,7 +22587,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="16">
+    <row r="104" spans="1:14" ht="15.75">
       <c r="A104" s="295"/>
       <c r="B104" s="83"/>
       <c r="C104" s="193"/>
@@ -22607,7 +22609,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="16">
+    <row r="105" spans="1:14" ht="15.75">
       <c r="A105" s="295"/>
       <c r="B105" s="83"/>
       <c r="C105" s="193"/>
@@ -22629,7 +22631,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="16">
+    <row r="106" spans="1:14" ht="15.75">
       <c r="A106" s="295"/>
       <c r="B106" s="83"/>
       <c r="C106" s="193"/>
@@ -22651,7 +22653,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="16">
+    <row r="107" spans="1:14" ht="15.75">
       <c r="A107" s="295"/>
       <c r="B107" s="83"/>
       <c r="C107" s="193"/>
@@ -22673,7 +22675,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="16">
+    <row r="108" spans="1:14" ht="15.75">
       <c r="A108" s="295"/>
       <c r="B108" s="83"/>
       <c r="C108" s="193"/>
@@ -22695,7 +22697,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="16">
+    <row r="109" spans="1:14" ht="15.75">
       <c r="A109" s="295"/>
       <c r="B109" s="83"/>
       <c r="C109" s="193"/>
@@ -22717,7 +22719,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="16">
+    <row r="110" spans="1:14" ht="15.75">
       <c r="A110" s="295"/>
       <c r="B110" s="83"/>
       <c r="C110" s="193"/>
@@ -22739,7 +22741,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="16">
+    <row r="111" spans="1:14" ht="15.75">
       <c r="A111" s="295"/>
       <c r="B111" s="83"/>
       <c r="C111" s="193"/>
@@ -22761,7 +22763,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="16">
+    <row r="112" spans="1:14" ht="15.75">
       <c r="A112" s="295"/>
       <c r="B112" s="83"/>
       <c r="C112" s="193"/>
@@ -22783,7 +22785,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="16">
+    <row r="113" spans="1:14" ht="15.75">
       <c r="A113" s="295"/>
       <c r="B113" s="83"/>
       <c r="C113" s="193"/>
@@ -22843,7 +22845,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="16">
+    <row r="115" spans="1:14" ht="15.75">
       <c r="A115" s="295"/>
       <c r="B115" s="83"/>
       <c r="C115" s="193"/>
@@ -22865,7 +22867,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="16">
+    <row r="116" spans="1:14" ht="15.75">
       <c r="A116" s="295"/>
       <c r="B116" s="83"/>
       <c r="C116" s="193"/>
@@ -22887,7 +22889,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="16">
+    <row r="117" spans="1:14" ht="15.75">
       <c r="A117" s="295"/>
       <c r="B117" s="83"/>
       <c r="C117" s="193"/>
@@ -22909,7 +22911,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="16">
+    <row r="118" spans="1:14" ht="15.75">
       <c r="A118" s="295"/>
       <c r="B118" s="83"/>
       <c r="C118" s="193"/>
@@ -22969,7 +22971,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="16">
+    <row r="120" spans="1:14" ht="15.75">
       <c r="A120" s="295"/>
       <c r="B120" s="83"/>
       <c r="C120" s="193"/>
@@ -22991,7 +22993,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="16">
+    <row r="121" spans="1:14" ht="15.75">
       <c r="A121" s="295"/>
       <c r="B121" s="83"/>
       <c r="C121" s="193"/>
@@ -23013,7 +23015,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="16">
+    <row r="122" spans="1:14" ht="15.75">
       <c r="A122" s="295"/>
       <c r="B122" s="83"/>
       <c r="C122" s="193"/>
@@ -23035,7 +23037,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="16">
+    <row r="123" spans="1:14" ht="15.75">
       <c r="A123" s="295"/>
       <c r="B123" s="83"/>
       <c r="C123" s="193"/>
@@ -23057,7 +23059,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="16">
+    <row r="124" spans="1:14" ht="15.75">
       <c r="A124" s="295"/>
       <c r="B124" s="83"/>
       <c r="C124" s="193"/>
@@ -23079,7 +23081,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="16">
+    <row r="125" spans="1:14" ht="15.75">
       <c r="A125" s="295"/>
       <c r="B125" s="83"/>
       <c r="C125" s="193"/>
@@ -23101,7 +23103,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="16">
+    <row r="126" spans="1:14" ht="15.75">
       <c r="A126" s="295"/>
       <c r="B126" s="83"/>
       <c r="C126" s="193"/>
@@ -23161,7 +23163,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="16">
+    <row r="128" spans="1:14" ht="15.75">
       <c r="A128" s="295"/>
       <c r="B128" s="83"/>
       <c r="C128" s="193"/>
@@ -23183,7 +23185,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="16">
+    <row r="129" spans="1:14" ht="15.75">
       <c r="A129" s="295"/>
       <c r="B129" s="83"/>
       <c r="C129" s="193"/>
@@ -23205,7 +23207,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="16">
+    <row r="130" spans="1:14" ht="15.75">
       <c r="A130" s="295"/>
       <c r="B130" s="83"/>
       <c r="C130" s="193"/>
@@ -23227,7 +23229,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="16">
+    <row r="131" spans="1:14" ht="15.75">
       <c r="A131" s="295"/>
       <c r="B131" s="83"/>
       <c r="C131" s="193"/>
@@ -23249,7 +23251,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="16">
+    <row r="132" spans="1:14" ht="15.75">
       <c r="A132" s="295"/>
       <c r="B132" s="83"/>
       <c r="C132" s="193"/>
@@ -23271,7 +23273,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="16">
+    <row r="133" spans="1:14" ht="15.75">
       <c r="A133" s="295"/>
       <c r="B133" s="83"/>
       <c r="C133" s="193"/>
@@ -23293,7 +23295,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="16">
+    <row r="134" spans="1:14" ht="15.75">
       <c r="A134" s="295"/>
       <c r="B134" s="83"/>
       <c r="C134" s="193"/>
@@ -23315,7 +23317,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="16">
+    <row r="135" spans="1:14" ht="15.75">
       <c r="A135" s="295"/>
       <c r="B135" s="83"/>
       <c r="C135" s="193"/>
@@ -23337,7 +23339,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="16">
+    <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="295"/>
       <c r="B136" s="83"/>
       <c r="C136" s="193"/>
@@ -23359,7 +23361,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="16">
+    <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="295"/>
       <c r="B137" s="83"/>
       <c r="C137" s="193"/>
@@ -23381,7 +23383,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="16">
+    <row r="138" spans="1:14" ht="15.75">
       <c r="A138" s="295"/>
       <c r="B138" s="83"/>
       <c r="C138" s="193"/>
@@ -23520,7 +23522,7 @@
       <c r="M142" s="66"/>
       <c r="N142" s="66"/>
     </row>
-    <row r="143" spans="1:14" ht="17">
+    <row r="143" spans="1:14" ht="15.75">
       <c r="A143" s="294"/>
       <c r="B143" s="93" t="s">
         <v>1644</v>
@@ -23546,7 +23548,7 @@
       <c r="M143" s="68"/>
       <c r="N143" s="68"/>
     </row>
-    <row r="144" spans="1:14" ht="17">
+    <row r="144" spans="1:14" ht="15.75">
       <c r="A144" s="294"/>
       <c r="B144" s="89" t="s">
         <v>1648</v>
@@ -23572,7 +23574,7 @@
       <c r="M144" s="68"/>
       <c r="N144" s="68"/>
     </row>
-    <row r="145" spans="1:14" ht="17">
+    <row r="145" spans="1:14" ht="15.75">
       <c r="A145" s="294"/>
       <c r="B145" s="89" t="s">
         <v>1652</v>
@@ -23604,7 +23606,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="17">
+    <row r="146" spans="1:14" ht="15.75">
       <c r="A146" s="294"/>
       <c r="B146" s="89"/>
       <c r="C146" s="193"/>
@@ -23626,7 +23628,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="17">
+    <row r="147" spans="1:14" ht="15.75">
       <c r="A147" s="294"/>
       <c r="B147" s="89"/>
       <c r="C147" s="193"/>
@@ -23648,7 +23650,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="17">
+    <row r="148" spans="1:14" ht="15.75">
       <c r="A148" s="294"/>
       <c r="B148" s="89"/>
       <c r="C148" s="193"/>
@@ -23670,7 +23672,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="17">
+    <row r="149" spans="1:14" ht="15.75">
       <c r="A149" s="294"/>
       <c r="B149" s="89"/>
       <c r="C149" s="193"/>
@@ -23692,7 +23694,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="17">
+    <row r="150" spans="1:14" ht="15.75">
       <c r="A150" s="294"/>
       <c r="B150" s="89"/>
       <c r="C150" s="193"/>
@@ -23714,7 +23716,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="17">
+    <row r="151" spans="1:14" ht="15.75">
       <c r="A151" s="294"/>
       <c r="B151" s="89"/>
       <c r="C151" s="193"/>
@@ -23736,7 +23738,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="17">
+    <row r="152" spans="1:14" ht="15.75">
       <c r="A152" s="294"/>
       <c r="B152" s="89"/>
       <c r="C152" s="193"/>
@@ -23758,7 +23760,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="17">
+    <row r="153" spans="1:14" ht="15.75">
       <c r="A153" s="294"/>
       <c r="B153" s="89"/>
       <c r="C153" s="193"/>
@@ -23780,7 +23782,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="17">
+    <row r="154" spans="1:14" ht="15.75">
       <c r="A154" s="294"/>
       <c r="B154" s="89"/>
       <c r="C154" s="193"/>
@@ -23802,7 +23804,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="17">
+    <row r="155" spans="1:14" ht="15.75">
       <c r="A155" s="294"/>
       <c r="B155" s="89"/>
       <c r="C155" s="193"/>
@@ -23824,7 +23826,7 @@
         <v>1688</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="17">
+    <row r="156" spans="1:14" ht="15.75">
       <c r="A156" s="294"/>
       <c r="B156" s="68"/>
       <c r="C156" s="68"/>
@@ -23846,7 +23848,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="17">
+    <row r="157" spans="1:14" ht="15.75">
       <c r="A157" s="294"/>
       <c r="B157" s="68"/>
       <c r="C157" s="68"/>
@@ -23868,7 +23870,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="17">
+    <row r="158" spans="1:14" ht="15.75">
       <c r="A158" s="294"/>
       <c r="B158" s="68"/>
       <c r="C158" s="68"/>
@@ -23890,7 +23892,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="17">
+    <row r="159" spans="1:14" ht="15.75">
       <c r="A159" s="294"/>
       <c r="B159" s="68"/>
       <c r="C159" s="68"/>
@@ -23912,7 +23914,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="17">
+    <row r="160" spans="1:14" ht="15.75">
       <c r="A160" s="294"/>
       <c r="B160" s="89" t="s">
         <v>1701</v>
@@ -23938,7 +23940,7 @@
       <c r="M160" s="68"/>
       <c r="N160" s="68"/>
     </row>
-    <row r="161" spans="1:14" ht="17">
+    <row r="161" spans="1:14" ht="15.75">
       <c r="A161" s="294"/>
       <c r="B161" s="89" t="s">
         <v>1705</v>
@@ -23982,27 +23984,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176E780C-1D59-4D93-8860-2965D1028317}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F18" workbookViewId="0">
+    <sheetView topLeftCell="F10" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="3" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.83203125" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="44.5" customWidth="1"/>
-    <col min="9" max="9" width="31.1640625" customWidth="1"/>
-    <col min="10" max="10" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="29.25">
       <c r="A1" s="79" t="s">
         <v>813</v>
       </c>
@@ -24165,7 +24167,7 @@
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
     </row>
-    <row r="6" spans="1:13" ht="32">
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" s="299"/>
       <c r="B6" s="245" t="s">
         <v>157</v>
@@ -24232,7 +24234,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="80">
+    <row r="8" spans="1:13" ht="75">
       <c r="A8" s="299"/>
       <c r="B8" s="245"/>
       <c r="C8" s="68"/>
@@ -24253,7 +24255,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="112">
+    <row r="9" spans="1:13" ht="105">
       <c r="A9" s="299"/>
       <c r="B9" s="245"/>
       <c r="C9" s="68"/>
@@ -24274,7 +24276,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="144">
+    <row r="10" spans="1:13" ht="105">
       <c r="A10" s="299"/>
       <c r="B10" s="245"/>
       <c r="C10" s="68"/>
@@ -24316,7 +24318,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16">
+    <row r="12" spans="1:13">
       <c r="A12" s="299"/>
       <c r="B12" s="245"/>
       <c r="C12" s="68"/>
@@ -24337,7 +24339,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16">
+    <row r="13" spans="1:13">
       <c r="A13" s="300"/>
       <c r="B13" s="245"/>
       <c r="C13" s="68"/>
@@ -24358,7 +24360,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="32">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="298" t="s">
         <v>1751</v>
       </c>
@@ -24434,7 +24436,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16">
+    <row r="16" spans="1:13">
       <c r="A16" s="299"/>
       <c r="B16" s="245"/>
       <c r="C16" s="68"/>
@@ -24455,7 +24457,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16">
+    <row r="17" spans="1:13">
       <c r="A17" s="299"/>
       <c r="B17" s="245"/>
       <c r="C17" s="68"/>
@@ -24634,7 +24636,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16">
+    <row r="24" spans="1:13">
       <c r="A24" s="299"/>
       <c r="B24" s="245"/>
       <c r="C24" s="68"/>
@@ -24868,26 +24870,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275C6F3D-C99D-47D9-BF3E-AC6E0C13AFAF}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="60" customWidth="1"/>
     <col min="2" max="3" width="35" style="60" customWidth="1"/>
-    <col min="4" max="4" width="43.83203125" style="60" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="60" customWidth="1"/>
-    <col min="6" max="7" width="26.5" style="60" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" style="60" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="60" customWidth="1"/>
+    <col min="6" max="7" width="26.42578125" style="60" customWidth="1"/>
     <col min="8" max="9" width="29" style="60" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" style="60" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="60" customWidth="1"/>
-    <col min="12" max="12" width="29.5" style="60" customWidth="1"/>
-    <col min="13" max="13" width="34.6640625" style="60" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="60"/>
+    <col min="10" max="10" width="21.85546875" style="60" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" style="60" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="60" customWidth="1"/>
+    <col min="13" max="13" width="34.5703125" style="60" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="147" t="s">
         <v>813</v>
       </c>
@@ -24928,7 +24930,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="119">
+    <row r="2" spans="1:13" ht="168.75">
       <c r="A2" s="301" t="s">
         <v>1820</v>
       </c>
@@ -25074,7 +25076,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="20.25">
       <c r="A8" s="301"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67"/>
@@ -25095,7 +25097,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="85">
+    <row r="9" spans="1:13" ht="120.75">
       <c r="A9" s="301"/>
       <c r="B9" s="67" t="s">
         <v>315</v>
@@ -25119,7 +25121,7 @@
         <v>1850</v>
       </c>
       <c r="I9" s="103" t="s">
-        <v>1428</v>
+        <v>2000</v>
       </c>
       <c r="J9" s="275" t="s">
         <v>1848</v>
@@ -25134,7 +25136,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21">
+    <row r="10" spans="1:13" ht="20.25">
       <c r="A10" s="301"/>
       <c r="B10" s="67"/>
       <c r="C10" s="67"/>
@@ -25192,7 +25194,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21">
+    <row r="12" spans="1:13" ht="20.25">
       <c r="A12" s="67"/>
       <c r="B12" s="67"/>
       <c r="C12" s="67"/>
@@ -25213,7 +25215,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16">
+    <row r="13" spans="1:13">
       <c r="A13" s="67"/>
       <c r="B13" s="67"/>
       <c r="C13" s="67"/>
@@ -25234,7 +25236,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="48">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="67"/>
       <c r="B14" s="67"/>
       <c r="C14" s="67"/>
@@ -25255,7 +25257,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16">
+    <row r="15" spans="1:13">
       <c r="A15" s="67"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -25276,7 +25278,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16">
+    <row r="16" spans="1:13">
       <c r="A16" s="67"/>
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
@@ -25297,7 +25299,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="48">
+    <row r="17" spans="1:13" ht="45">
       <c r="A17" s="67"/>
       <c r="B17" s="67"/>
       <c r="C17" s="67"/>
@@ -25318,7 +25320,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="48">
+    <row r="18" spans="1:13" ht="45">
       <c r="A18" s="67"/>
       <c r="B18" s="67"/>
       <c r="C18" s="67"/>
@@ -25339,7 +25341,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="32">
+    <row r="19" spans="1:13" ht="30">
       <c r="A19" s="67"/>
       <c r="B19" s="67"/>
       <c r="C19" s="67"/>
@@ -25360,7 +25362,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16">
+    <row r="20" spans="1:13">
       <c r="A20" s="67"/>
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
@@ -25381,7 +25383,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16">
+    <row r="21" spans="1:13">
       <c r="A21" s="67"/>
       <c r="B21" s="67"/>
       <c r="C21" s="67"/>
@@ -25474,7 +25476,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17">
+    <row r="24" spans="1:13" ht="15.75">
       <c r="A24" s="301"/>
       <c r="B24" s="67"/>
       <c r="C24" s="67"/>
@@ -25495,7 +25497,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="17">
+    <row r="25" spans="1:13" ht="15.75">
       <c r="A25" s="301"/>
       <c r="B25" s="67"/>
       <c r="C25" s="67"/>
@@ -25516,7 +25518,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17">
+    <row r="26" spans="1:13" ht="15.75">
       <c r="A26" s="301"/>
       <c r="B26" s="67"/>
       <c r="C26" s="67"/>
@@ -25537,7 +25539,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17">
+    <row r="27" spans="1:13" ht="15.75">
       <c r="A27" s="301"/>
       <c r="B27" s="67"/>
       <c r="C27" s="67"/>
@@ -25558,7 +25560,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17">
+    <row r="28" spans="1:13" ht="15.75">
       <c r="A28" s="301"/>
       <c r="B28" s="67"/>
       <c r="C28" s="67"/>
@@ -25579,7 +25581,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17">
+    <row r="29" spans="1:13" ht="15.75">
       <c r="A29" s="301"/>
       <c r="B29" s="67"/>
       <c r="C29" s="67"/>
@@ -25618,7 +25620,7 @@
         <v>1918</v>
       </c>
       <c r="I30" s="67" t="s">
-        <v>1428</v>
+        <v>2000</v>
       </c>
       <c r="J30" s="67"/>
       <c r="K30" s="115" t="s">
@@ -25631,7 +25633,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16">
+    <row r="31" spans="1:13">
       <c r="A31" s="301"/>
       <c r="B31" s="67"/>
       <c r="C31" s="67"/>
@@ -25676,7 +25678,7 @@
         <v>1922</v>
       </c>
       <c r="I32" s="67" t="s">
-        <v>1428</v>
+        <v>2000</v>
       </c>
       <c r="J32" s="275" t="s">
         <v>1923</v>
@@ -25691,7 +25693,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16">
+    <row r="33" spans="1:13">
       <c r="A33" s="301"/>
       <c r="B33" s="67"/>
       <c r="C33" s="67"/>
@@ -25767,7 +25769,7 @@
         <v>1931</v>
       </c>
       <c r="I35" s="67" t="s">
-        <v>1428</v>
+        <v>2000</v>
       </c>
       <c r="J35" s="275" t="s">
         <v>1932</v>
@@ -25782,7 +25784,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16">
+    <row r="36" spans="1:13">
       <c r="A36" s="301"/>
       <c r="B36" s="67"/>
       <c r="C36" s="67"/>
@@ -25834,6 +25836,7 @@
     <mergeCell ref="A22:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -25845,23 +25848,22 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.1640625" customWidth="1"/>
-    <col min="8" max="9" width="18.1640625" customWidth="1"/>
-    <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="11" width="35.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="44.140625" customWidth="1"/>
+    <col min="8" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
     <col min="12" max="12" width="39" customWidth="1"/>
-    <col min="13" max="13" width="63.5" customWidth="1"/>
+    <col min="13" max="13" width="63.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
@@ -25940,7 +25942,7 @@
       </c>
       <c r="N2" s="273"/>
     </row>
-    <row r="3" spans="1:14" ht="16">
+    <row r="3" spans="1:14" ht="17.25">
       <c r="A3" s="68"/>
       <c r="B3" s="269"/>
       <c r="C3" s="269"/>
@@ -25962,7 +25964,7 @@
       </c>
       <c r="N3" s="273"/>
     </row>
-    <row r="4" spans="1:14" ht="17">
+    <row r="4" spans="1:14" ht="17.25">
       <c r="A4" s="68"/>
       <c r="B4" s="269"/>
       <c r="C4" s="269"/>
@@ -25984,7 +25986,7 @@
       </c>
       <c r="N4" s="273"/>
     </row>
-    <row r="5" spans="1:14" ht="17">
+    <row r="5" spans="1:14" ht="17.25">
       <c r="A5" s="68"/>
       <c r="B5" s="269"/>
       <c r="C5" s="269"/>
@@ -26006,7 +26008,7 @@
       </c>
       <c r="N5" s="273"/>
     </row>
-    <row r="6" spans="1:14" ht="17">
+    <row r="6" spans="1:14" ht="32.25">
       <c r="A6" s="68"/>
       <c r="B6" s="269"/>
       <c r="C6" s="269"/>
@@ -26028,7 +26030,7 @@
       </c>
       <c r="N6" s="273"/>
     </row>
-    <row r="7" spans="1:14" ht="17">
+    <row r="7" spans="1:14" ht="17.25">
       <c r="A7" s="68"/>
       <c r="B7" s="269"/>
       <c r="C7" s="269"/>
@@ -26050,7 +26052,7 @@
       </c>
       <c r="N7" s="273"/>
     </row>
-    <row r="8" spans="1:14" ht="17">
+    <row r="8" spans="1:14" ht="17.25">
       <c r="A8" s="68"/>
       <c r="B8" s="269"/>
       <c r="C8" s="269"/>
@@ -26072,7 +26074,7 @@
       </c>
       <c r="N8" s="273"/>
     </row>
-    <row r="9" spans="1:14" ht="16">
+    <row r="9" spans="1:14" ht="17.25">
       <c r="A9" s="68"/>
       <c r="B9" s="269"/>
       <c r="C9" s="269"/>
@@ -26132,7 +26134,7 @@
       </c>
       <c r="N10" s="274"/>
     </row>
-    <row r="11" spans="1:14" ht="16">
+    <row r="11" spans="1:14" ht="17.25">
       <c r="A11" s="68"/>
       <c r="B11" s="272"/>
       <c r="C11" s="272"/>
@@ -26154,7 +26156,7 @@
       </c>
       <c r="N11" s="274"/>
     </row>
-    <row r="12" spans="1:14" ht="16">
+    <row r="12" spans="1:14" ht="17.25">
       <c r="A12" s="68"/>
       <c r="B12" s="272"/>
       <c r="C12" s="272"/>
@@ -26176,7 +26178,7 @@
       </c>
       <c r="N12" s="274"/>
     </row>
-    <row r="13" spans="1:14" ht="16">
+    <row r="13" spans="1:14" ht="17.25">
       <c r="A13" s="68"/>
       <c r="B13" s="272"/>
       <c r="C13" s="272"/>
@@ -26198,7 +26200,7 @@
       </c>
       <c r="N13" s="274"/>
     </row>
-    <row r="14" spans="1:14" ht="16">
+    <row r="14" spans="1:14" ht="17.25">
       <c r="A14" s="68"/>
       <c r="B14" s="272"/>
       <c r="C14" s="272"/>
@@ -26220,7 +26222,7 @@
       </c>
       <c r="N14" s="274"/>
     </row>
-    <row r="15" spans="1:14" ht="16">
+    <row r="15" spans="1:14" ht="17.25">
       <c r="A15" s="68"/>
       <c r="B15" s="272"/>
       <c r="C15" s="272"/>
@@ -26242,7 +26244,7 @@
       </c>
       <c r="N15" s="274"/>
     </row>
-    <row r="16" spans="1:14" ht="16">
+    <row r="16" spans="1:14" ht="17.25">
       <c r="A16" s="68"/>
       <c r="B16" s="272"/>
       <c r="C16" s="272"/>
@@ -26264,7 +26266,7 @@
       </c>
       <c r="N16" s="274"/>
     </row>
-    <row r="17" spans="1:14" ht="16">
+    <row r="17" spans="1:14" ht="17.25">
       <c r="A17" s="68"/>
       <c r="B17" s="272"/>
       <c r="C17" s="272"/>
@@ -26286,7 +26288,7 @@
       </c>
       <c r="N17" s="274"/>
     </row>
-    <row r="18" spans="1:14" ht="16">
+    <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="68"/>
       <c r="B18" s="272"/>
       <c r="C18" s="272"/>
@@ -26314,6 +26316,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00591925-1995-4bf8-8d28-1f7cbeda4924">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A595C2436754DD4192B3BEE0FFE1ED0A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93ba19257e65125414350f132367e985">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00591925-1995-4bf8-8d28-1f7cbeda4924" xmlns:ns3="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2a6491f746e84da8ae5f2642b9bcf21" ns2:_="" ns3:_="">
     <xsd:import namespace="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
@@ -26542,7 +26555,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -26551,18 +26564,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00591925-1995-4bf8-8d28-1f7cbeda4924">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{319AAEED-380C-474B-BD5E-BD614C666CFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d"/>
+    <ds:schemaRef ds:uri="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72B4B015-2F19-4BB0-A14D-E91581C50494}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26581,21 +26594,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32FAF7A7-D9AD-4A85-9EE8-33F1ACC4911B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{319AAEED-380C-474B-BD5E-BD614C666CFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d"/>
-    <ds:schemaRef ds:uri="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>